<commit_message>
Update web app mode dir Update Datset metadata
</commit_message>
<xml_diff>
--- a/Dataset metadata.xlsx
+++ b/Dataset metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\Plant-Leaf-Disease-Classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE64D752-7301-4359-867F-559589281138}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F935E897-707E-46E6-9989-6609E6E458AE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1785" yWindow="720" windowWidth="18975" windowHeight="9225" xr2:uid="{35E35657-BE11-40BB-8B35-5D4935A9B321}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{35E35657-BE11-40BB-8B35-5D4935A9B321}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Nama Daun</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Yellow Leaf Curl Virus</t>
   </si>
   <si>
-    <t>Mosaic Virus</t>
-  </si>
-  <si>
     <t>Bacterial spot</t>
   </si>
   <si>
@@ -99,7 +96,13 @@
     <t>Jumlah</t>
   </si>
   <si>
-    <t>Common rust</t>
+    <t>Common rust_</t>
+  </si>
+  <si>
+    <t>Early Blight</t>
+  </si>
+  <si>
+    <t>Mosaic virus</t>
   </si>
 </sst>
 </file>
@@ -259,8 +262,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -273,22 +292,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC48A15-2F8F-4E38-B179-0520A5BCD4D0}">
-  <dimension ref="B2:E22"/>
+  <dimension ref="B2:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,178 +633,220 @@
   <sheetData>
     <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="2"/>
+      <c r="D3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="12"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5" t="s">
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="7" t="s">
+      <c r="B5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="8"/>
+      <c r="D5" s="15">
+        <v>410</v>
+      </c>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="9"/>
-      <c r="C6" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="11"/>
+      <c r="C6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="16">
+        <v>500</v>
+      </c>
+      <c r="E6" s="5"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="9"/>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="11"/>
+      <c r="D7" s="16">
+        <v>500</v>
+      </c>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="12"/>
-      <c r="C8" s="13" t="s">
+      <c r="B8" s="10"/>
+      <c r="C8" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="14"/>
+      <c r="D8" s="17">
+        <v>500</v>
+      </c>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="7" t="s">
+      <c r="B9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="8"/>
+      <c r="D9" s="15">
+        <v>500</v>
+      </c>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="9"/>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="11"/>
+      <c r="D10" s="16">
+        <v>500</v>
+      </c>
+      <c r="E10" s="5"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="12"/>
-      <c r="C11" s="13" t="s">
+      <c r="B11" s="10"/>
+      <c r="C11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="14"/>
+      <c r="D11" s="17">
+        <v>121</v>
+      </c>
+      <c r="E11" s="7"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="7" t="s">
+      <c r="B12" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="8"/>
+      <c r="C12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="15">
+        <v>500</v>
+      </c>
+      <c r="E12" s="3"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="9"/>
-      <c r="C13" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="11"/>
+      <c r="C13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="16">
+        <v>500</v>
+      </c>
+      <c r="E13" s="5"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="9"/>
-      <c r="C14" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="11"/>
+      <c r="C14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="16">
+        <v>500</v>
+      </c>
+      <c r="E14" s="5"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="9"/>
-      <c r="C15" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="11"/>
+      <c r="C15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="16">
+        <v>500</v>
+      </c>
+      <c r="E15" s="5"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="9"/>
-      <c r="C16" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="11"/>
+      <c r="C16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="16">
+        <v>500</v>
+      </c>
+      <c r="E16" s="5"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="9"/>
-      <c r="C17" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="11"/>
+      <c r="C17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="16">
+        <v>500</v>
+      </c>
+      <c r="E17" s="5"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="9"/>
-      <c r="C18" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="11"/>
+      <c r="C18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="16">
+        <v>500</v>
+      </c>
+      <c r="E18" s="5"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="9"/>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="16">
+        <v>299</v>
+      </c>
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="10"/>
+      <c r="C20" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="17">
+        <v>500</v>
+      </c>
+      <c r="E20" s="7"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="15">
+        <v>500</v>
+      </c>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="10"/>
+      <c r="C22" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="11"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="12"/>
-      <c r="C20" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="14"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="8"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="12"/>
-      <c r="C22" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="14"/>
+      <c r="D22" s="17">
+        <v>500</v>
+      </c>
+      <c r="E22" s="7"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <f>SUM(D5:D22)</f>
+        <v>8330</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>